<commit_message>
Added basic inventory management along with inventory GUI/map changes
</commit_message>
<xml_diff>
--- a/mapDef.xlsx
+++ b/mapDef.xlsx
@@ -2070,7 +2070,7 @@
   <dimension ref="A1:Y25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2255,7 +2255,7 @@
         <v>-1</v>
       </c>
       <c r="H3" s="0" t="n">
-        <v>-1</v>
+        <v>68</v>
       </c>
       <c r="I3" s="0" t="n">
         <v>-1</v>
@@ -2939,7 +2939,7 @@
         <v>-1</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>-1</v>
+        <v>68</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>-1</v>
@@ -2963,7 +2963,7 @@
         <v>-1</v>
       </c>
       <c r="M12" s="0" t="n">
-        <v>-1</v>
+        <v>68</v>
       </c>
       <c r="N12" s="0" t="n">
         <v>-1</v>
@@ -3312,31 +3312,31 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>-1</v>
+        <v>68</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>68</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>58</v>
+        <v>-1</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>-1</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>-1</v>
+        <v>68</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>-1</v>
       </c>
       <c r="G17" s="0" t="n">
-        <v>-1</v>
+        <v>68</v>
       </c>
       <c r="H17" s="0" t="n">
         <v>-1</v>
       </c>
       <c r="I17" s="0" t="n">
-        <v>-1</v>
+        <v>68</v>
       </c>
       <c r="J17" s="0" t="n">
         <v>-1</v>
@@ -3392,7 +3392,7 @@
         <v>-1</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>-1</v>
+        <v>69</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>-1</v>

</xml_diff>

<commit_message>
Refactor to follow PEP8 coding standard
</commit_message>
<xml_diff>
--- a/mapDef.xlsx
+++ b/mapDef.xlsx
@@ -121,7 +121,7 @@
       <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
@@ -2070,10 +2070,10 @@
   <dimension ref="A1:Y25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
@@ -2619,7 +2619,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>-1</v>
+        <v>69</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>-1</v>
@@ -2850,13 +2850,13 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>-1</v>
+        <v>69</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>-1</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>-1</v>
+        <v>69</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>-1</v>
@@ -2865,10 +2865,10 @@
         <v>-1</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>-1</v>
+        <v>70</v>
       </c>
       <c r="G11" s="0" t="n">
-        <v>-1</v>
+        <v>71</v>
       </c>
       <c r="H11" s="0" t="n">
         <v>-1</v>
@@ -2942,10 +2942,10 @@
         <v>68</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>-1</v>
+        <v>78</v>
       </c>
       <c r="G12" s="0" t="n">
-        <v>-1</v>
+        <v>79</v>
       </c>
       <c r="H12" s="0" t="n">
         <v>-1</v>
@@ -4025,7 +4025,7 @@
       <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
@@ -5977,7 +5977,7 @@
       <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>

</xml_diff>

<commit_message>
Adding comments and approaching pep8 standard
</commit_message>
<xml_diff>
--- a/mapDef.xlsx
+++ b/mapDef.xlsx
@@ -33,7 +33,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2070,7 +2069,7 @@
   <dimension ref="A1:Y25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3096,7 +3095,7 @@
         <v>-1</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>-1</v>
+        <v>44</v>
       </c>
       <c r="G14" s="0" t="n">
         <v>-1</v>
@@ -3179,10 +3178,10 @@
         <v>-1</v>
       </c>
       <c r="H15" s="0" t="n">
-        <v>-1</v>
+        <v>62</v>
       </c>
       <c r="I15" s="0" t="n">
-        <v>-1</v>
+        <v>63</v>
       </c>
       <c r="J15" s="0" t="n">
         <v>-1</v>

</xml_diff>